<commit_message>
added ProductIssue complete CRUD with controller, service, repo etc
</commit_message>
<xml_diff>
--- a/employee.xlsx
+++ b/employee.xlsx
@@ -7,6 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Small Sheet" r:id="rId3" sheetId="1"/>
+    <sheet name="Sheet2" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
@@ -105,4 +106,16 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>